<commit_message>
add area to Q files stn5
</commit_message>
<xml_diff>
--- a/Discharge/Station5_2021-06-11_1248.xlsx
+++ b/Discharge/Station5_2021-06-11_1248.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tessamd\Desktop\Ecuador Discharge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A41610D2D507EE013333539B014CB0AD2039895A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7753251E-5894-4E31-BB02-8AB696450476}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14640" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -43,11 +53,17 @@
   <si>
     <t>Qtotal</t>
   </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Atotal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,16 +374,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +402,20 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>80</v>
       </c>
@@ -405,8 +433,24 @@
         <f>SUM(E2:E20)</f>
         <v>4.7080000000000011E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <f>(D2-0)*B2/100</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(G2:G11)</f>
+        <v>0.21800000000000003</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>0.21800000000000003</v>
+      </c>
+      <c r="K2">
+        <f>F2</f>
+        <v>4.7080000000000011E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>90</v>
       </c>
@@ -424,8 +468,12 @@
         <f t="shared" ref="E3:E19" si="0">(D3-D2)*(B3/100)*C3</f>
         <v>-1.7999999999999991E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <f>(D3-D2)*B3/100</f>
+        <v>2.9999999999999982E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>100</v>
       </c>
@@ -443,8 +491,12 @@
         <f t="shared" si="0"/>
         <v>5.600000000000006E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <f t="shared" ref="G4:G15" si="1">(D4-D3)*B4/100</f>
+        <v>2.8000000000000025E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>110</v>
       </c>
@@ -462,8 +514,12 @@
         <f>(D5-D4)*(B5/100)*C5</f>
         <v>6.3999999999999925E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>3.1999999999999959E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>120</v>
       </c>
@@ -474,15 +530,19 @@
         <v>0.23</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D19" si="1">(A6/100+(A7/100-A6/100)/2)</f>
+        <f t="shared" ref="D6:D19" si="2">(A6/100+(A7/100-A6/100)/2)</f>
         <v>1.25</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>7.3600000000000072E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000028E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>130</v>
       </c>
@@ -493,15 +553,19 @@
         <v>0.34</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>1.6319999999999991E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4.7999999999999973E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>150</v>
       </c>
@@ -512,15 +576,19 @@
         <v>0.38</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.55</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>1.8240000000000017E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000043E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>160</v>
       </c>
@@ -531,77 +599,105 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -611,7 +707,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -621,7 +717,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -631,7 +727,7 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E19">

</xml_diff>